<commit_message>
Switching machines - WIP
</commit_message>
<xml_diff>
--- a/xls/todo.xlsx
+++ b/xls/todo.xlsx
@@ -1,31 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Demuyt\Desktop\Portable\wsx\xls\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50B04497-7F03-4F9E-B6A3-6BA23B8269FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
-    <sheet name="tasks" sheetId="1" r:id="rId1"/>
+    <sheet state="visible" name="Items" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="No Items" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Blank" sheetId="3" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="18">
   <si>
     <t>ID</t>
   </si>
@@ -68,25 +56,47 @@
   <si>
     <t>URLs</t>
   </si>
+  <si>
+    <t>Finish PEW</t>
+  </si>
+  <si>
+    <t>Almost done</t>
+  </si>
+  <si>
+    <t>This is a note</t>
+  </si>
+  <si>
+    <t>Example</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
+  </numFmts>
+  <fonts count="4">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <sz val="10.0"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="Arial"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -95,152 +105,102 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="lightGray"/>
     </fill>
   </fills>
   <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+  <cellXfs count="5">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Sheets">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="000000"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4285F4"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="EA4335"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="FBBC04"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="34A853"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="FF6D01"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="46BDC6"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="1155CC"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="1155CC"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Sheets">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:latin typeface="Arial"/>
+        <a:ea typeface="Arial"/>
+        <a:cs typeface="Arial"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:latin typeface="Arial"/>
+        <a:ea typeface="Arial"/>
+        <a:cs typeface="Arial"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -381,82 +341,163 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.28515625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D2" s="4">
+        <v>45748.0</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="4">
+        <v>45413.0</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
-<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
-  <clbl:label id="{2590e1b2-66ea-4d45-b1aa-185c322e3ba5}" enabled="1" method="Standard" siteId="{40a64d0b-f2f9-4a34-b1b3-0992ac0e5e4e}" contentBits="0" removed="0"/>
-</clbl:labelList>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>